<commit_message>
latest update of changes
</commit_message>
<xml_diff>
--- a/src/main/resources/data/exceldata.xlsx
+++ b/src/main/resources/data/exceldata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knasurudeen\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knasurudeen\git\Training-Course\Quantum_IAP_Framwork\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8BC83A8-44AB-45AF-9091-3D8D8C087F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{951F4C78-EF8B-4EBF-A447-CAD9CC70A9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F5CCC561-5DB4-4E00-8412-BE24EC536C30}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>firstname</t>
   </si>
@@ -66,6 +66,30 @@
   </si>
   <si>
     <t>Others</t>
+  </si>
+  <si>
+    <t>Joel</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>ydg@hotmail.com</t>
+  </si>
+  <si>
+    <t>Neel</t>
+  </si>
+  <si>
+    <t>Kill</t>
+  </si>
+  <si>
+    <t>Dustin</t>
+  </si>
+  <si>
+    <t>Selenium Automation</t>
+  </si>
+  <si>
+    <t>Mobile Automation</t>
   </si>
 </sst>
 </file>
@@ -132,13 +156,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -454,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD35BB2B-CEC6-404E-8CCA-E0F99D9B96D5}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,11 +528,83 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{8AC32605-B6E9-437D-B2B9-3F2B0237F3DA}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{E5DB138A-DDE6-47DA-9DF4-F8D84A3D788E}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{956771DC-A9FB-440B-B1D1-ACAF218C1E06}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{43B88FF1-5078-496D-BBEE-A7C9DD52A5D5}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{735280C4-CCB7-4B7E-A345-A029FE15C669}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>